<commit_message>
Get daily reddit data: Tue Jan 16 08:08:28 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_21.xlsx
+++ b/data/2024_01_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C458"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2675 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>197xgjs</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Oh no</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/197xgjs/oh_no/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>197x8vm</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Winter nails. Sweater design with matte finish.</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlki926c9rcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>197x67p</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>How would you rate it…? Swipe right to see the picture I provided.</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197x67p</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>197vcuf</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>First time taking the time to do my own nails. I feel like they're very childish, but it was worth a shot. Trying to grow out my nails, so I used a gel overlay</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/habuixljpqcc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>197uyuu</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Press on set from Ulta!</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib0pxy4plqcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>197ty4f</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>My attempt at the tarnished silver look.</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197ty4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>197txxo</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>How to properly use nail strengthener?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/197txxo/how_to_properly_use_nail_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>197t728</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>first time getting cat eye nails</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dma91pj5qcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>197rotv</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>are my nails too thin to put acrylics on?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197rotv</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>197rm91</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>CAT NAILS!!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197rm91</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>197sjta</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Tried chrome for the first time!</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197sjta</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>197rwzq</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Channeling spring with purple 💜</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rn6fs20aupcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>197rceg</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Rager by I Scream Nails in da sunshine</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5ez8gtdppcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>197r9vj</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>I need the toughest top coat I can get that won't break the bank.</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/197r9vj/i_need_the_toughest_top_coat_i_can_get_that_wont/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>197r4qq</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Rubber base questions</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/197r4qq/rubber_base_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>197qt0c</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>help with small nails</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/197qt0c/help_with_small_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>197qq7b</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Weak nails</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/197qq7b/weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>197q78l</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Got a pastel French mani today!</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9d6px1izfpcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>197q1v1</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Fun Mani</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197q1v1</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>197prkv</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Flowers 🌺 with a Touch of Green</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qysnu8oecpcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>197oxgw</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>New nails, new vibes, same love for this color! 💅✨</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jif3iec5pcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>197oqiu</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Simplicity for me…. 🩶🤍🩶</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cloo2bk24pcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>197om8t</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Working on my technique</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5d4u4n143pcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>197ie5a</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Please ignore my dry ass hands, it's 12° outside</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197ie5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>197i6hp</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Set inspired by glass beads</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197i6hp</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>197nocq</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Held versus polygel</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/197nocq/held_versus_polygel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>197nj18</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>gel polish lifting after hand washing?</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/197nj18/gel_polish_lifting_after_hand_washing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>197d4bc</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Toenail Question</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/197d4bc/toenail_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>197goqo</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>what shape should i file my nails to suit me?</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197goqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>197nbed</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>9 weeks of no biting!! &lt;3</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197nbed</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>197n6uy</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Tried out the bobby pin cat eye hearts ♥️</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yk06mjzsrocc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>197moto</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>i have dermatillomania, and got acrylic nails done 1 week ago, are there any tips from people who are/went through dermatillomania (specifically the nails, and skin around the nails?)</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197moto</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>197m5sz</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Just reposting because my previous post got deleted :( but here’s my latest set, first time getting something so dark!</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197m5sz</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>197lqin</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Cat eye 🤝 chrome</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iajshk2shocc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>197l29n</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>first time doing a dip manicure on myself! idk how to feel about the melon color…🫨</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uda3u0p5docc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>197k8vk</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>my natural nails after 3 months without cutting them</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqo60z4b7occ1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>197k6m4</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Still learning</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvtfv3c07occ1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>197k104</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Help quick fix for nails</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/197k104/help_quick_fix_for_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>197k0n5</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>First time doing gel X DIY</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197k0n5</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>197jwx0</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Just some simple red nails. c: Would love some tips on how to prevent chipping! ❤️</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9utptz45occ1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>197jayj</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>This might be my favorite set I’ve done thus far</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dr3ywg2z0occ1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>197j46b</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>First attempt at cheetah nails… giving snow leopard</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvklp8vozncc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>197irzs</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Should I try coffin nails? Tried a classic red, taking a break from designs this week to focus on class. (◍´ᯅ `◍) 🦞❤️</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197irzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1972iw4</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>How do I improve my nails' health?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3c5slh0zxjcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1972b81</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Help please &lt;3</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1972b81/help_please_3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>197inhl</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>My real nails!! for my birthday!!! Oval shape with structure gel one hand chrome and the other is velvet cat eye. done by _stylesbylydia Methuen, MA, USA. she’s so sweet 🩷💙</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197inhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>197iio3</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Broken nails:(</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197iio3</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>197ifjp</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Saving money because you can do your own nails 😃 waiting between sets to do them again 😢</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nld5s8exuncc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>197i78b</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Ridges in nails</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197i78b</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>197cp5x</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>For people with long nails, how do you use your hands without them popping off?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/197cp5x/for_people_with_long_nails_how_do_you_use_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>197htr1</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Cold jojoba oil</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/197htr1/cold_jojoba_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>197h4up</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Anyone else grow their nails long but keep just their thumbs short? 😂 it’s really practical for phone usage imo</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zcstjovlncc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>197gtou</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>My first "fancy" Nail art</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7s77mw4qjncc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>197gs7k</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>What do you think of this press on nail set?</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62ipjvkfjncc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>197fix3</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Dreaming of Spring 🌱 -- Essie Expressie "Express to Impress"</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197fix3</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>197fd07</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Birthday Set</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kdlv00bq9ncc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>197f8ar</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Glowing galaxy🪐🌟</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhas781t8ncc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1970jnr</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Storing Gel Polish in the Cold</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1970jnr/storing_gel_polish_in_the_cold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1970exf</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>First Gel X set at home</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ttghw51bcjcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>196yr0g</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Soft gel under hard gel?</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/196yr0g/soft_gel_under_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>196yi2n</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Favorite hand and nail cream?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/196yi2n/favorite_hand_and_nail_cream/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>196wcyd</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Fixing Nails after Dip</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/196wcyd/fixing_nails_after_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>196w2y8</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>how to get stronger nails?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/196w2y8/how_to_get_stronger_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>197dw4z</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>delicate and sophisticated nalis</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nnfqj8dzmcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>197dmiv</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>I love my short natural nails 😍</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecx3vbiixmcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>197di4w</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>This color is perfect for the summer! And I also love the flowers they gave me</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2zikjdmwmcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>197ddlu</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Ok I’m officially an Apres/Gel X convert…….</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197ddlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>197czkk</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Valentine's is my favourite time of year for nails so I started early with a subtle lil accent heart 🤍</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nzpkl4xsmcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>197ckkx</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>What do you think of my nails?🩷</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icbpig4zpmcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>197cfzh</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>I know they're not extremely long but I'm proud of my nails</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197cfzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>197bxwf</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>I can't wait to use these!! ✨💖✨</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xxnv1muclmcc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>197bq6a</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>I really like these nails</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cx8zlsesjmcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>197bhd0</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Finally stopped biting my nails !</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197bhd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>197a9hn</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>I'm obsessed with my nails</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/197a9hn/im_obsessed_with_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1979g08</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Te las harías ?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvacjeax1mcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>197992c</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izbi542c0mcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>19794o8</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Copying @nuocmamkimchi</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ve9mgzt8zlcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1978bf9</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Seeking Recommendations: Which Nail System Should I Use for At-Home Manicures?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1978bf9/seeking_recommendations_which_nail_system_should/</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1977zst</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Nail amateur with gel nails</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cd10mthzolcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1977wov</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Gap between my nails and my gel</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1977wov/gap_between_my_nails_and_my_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1977v2x</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>engagement nails🤍💍🕊️</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wse6edponlcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>19776x4</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Watched Mean Girls with my teen and her friend, had a nail party. I'm in love with this glitter.</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19776x4</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1976qzo</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Bold and beautiful in red 💅</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/serupnxqblcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>19753l0</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Colorful French nails</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4fkz38vskcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>197401o</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Doing my Nails a little bit over a year - the newest!</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g92i182afkcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1973u16</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>My nails after…what can I do?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1973u16</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>197wqbm</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>I only started doing my own nails in November 🙊</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/haj4gcsi3rcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>197vtal</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Working with Magnets &amp; Magnetics</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197vtal</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>197un06</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>First Nail Art Attempt</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197un06</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>197sxrk</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Snowy Jelly Nails</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kv9ez583qcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>197sx8y</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Tried the magnetic heart hack with regular polish!</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u5ran9633qcc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>197sjvo</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Tawny</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/197sjvo/tawny/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>197s4cj</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Swatch Questions</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/197s4cj/swatch_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>197rjn6</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>First foil</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197rjn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>197rdlk</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Peel-Off Nail Polish</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/197rdlk/peeloff_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>197rcnj</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Rager by I Scream Nails in da sunshine</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q1a757zfppcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>197q0j1</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Loving this combination</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197q0j1</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>197puse</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>BKL - His Gentle Ruler</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197puse</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>197phnh</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Glass jellyfish in the freezer at work😂👌🏻🩷✨</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gmrewg76apcc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>197pcuh</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Back to doing my own nails after 1.5 year hiatus 🙌</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gh81u839pcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>197owrd</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Dam Polish Data Is My Love Language ✨️</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197owrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>197or8p</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>First ILNP haul 😍✨</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197or8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>197o769</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Base Alternative to OPI Nail Envy?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/197o769/base_alternative_to_opi_nail_envy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>197egep</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Thoughts on Manucurist Green Flash?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/197egep/thoughts_on_manucurist_green_flash/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>197np3w</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Seche Vite and nail vinyls</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/197np3w/seche_vite_and_nail_vinyls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>197mccn</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Fairy Dust 🧚🏻‍♀️✨</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197mccn</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>197m1th</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>RIP in Pieces</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197m1th</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>197lwc4</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Swipe for glow up ➡️</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197lwc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>197lsx5</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>A fiery franken for the cold weather</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7h3tcfu9iocc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>197l95t</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Will my proximal nail fold reattach? Salon drilled it off</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197l95t</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>197l54k</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Cupcake Polish Mom Jeans, ft. my actual jeans</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2o3gtw4pdocc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>197krdc</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Nail art🌊</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197krdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>197k9my</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>ILNP's Cake Pop</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mw1qujrk7occ1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>197k89c</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>What is your ugliest or your most disliked polish/es in your collection?</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/197k89c/what_is_your_ugliest_or_your_most_disliked/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>197jzsj</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Mooncat</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/197jzsj/mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>197j2ul</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Cygnus loop ❤️💙</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197j2ul</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>197j0ts</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Feeling sparkly!</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fuwpycl1zncc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>197iqb9</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>I know these are bad, but it's my first time after more than a year so be gentle :)</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8v30jpf0xncc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>197i438</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>🔥Hot Gradient🔥</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197i438</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>197i19w</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Finally bought in on House of Hades</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/or50vla7sncc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>197hwn7</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Feeling blue this season!</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v358fb1crncc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>197gxry</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Patience is a virtue! Self-mixed jelly nude plus green dots that didn’t quite dry before topcoat</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197gxry</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>197ghrc</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Refreshed Mani</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197ghrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>197fqgh</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Feeling colorful today</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1jt5as9cncc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>197fmpd</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>I’m obsessed! I used OPI Cozu-Melted in the Sun and Holotaco Polar princess with OPI rapid dry top coat and natural nail base coat.</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jdl4oemkbncc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>197etzc</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Cirque BAE; velvetized</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197etzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>197eisu</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>One week of wear on Elsa</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qov5fu0t3ncc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>197e2uv</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Polish Storage Suggestions Needed</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/197e2uv/polish_storage_suggestions_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>197d444</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>ILNP Dakota</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197d444</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>197cb4f</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Skittles Ombre Jellies</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197cb4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>197c1bz</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Did my very first Gel X set!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kw7j0e26mmcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>197c191</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>ISO frostbitten/bluberry milk crelly</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/197c191/iso_frostbittenbluberry_milk_crelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>197bsaz</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Finally Paying Cat Tax</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o8dv8u69kmcc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>197bqqr</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Inspired by my toddler’s favorite ball</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197bqqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>197bd3f</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>It so looks like it has its own light source</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197bd3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>197b6f6</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>It's very cold today, time for a cool jelly! Orly bonder, Picture Polish - North Pole, Seche Vite</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tts3c5affmcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>197aigd</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>What the shell?!</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197aigd</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>19781m6</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Reflective AND Regular Glitter?!</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jjgbtkweplcc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1977kok</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Was I supposed to use the magnetic wand before applying the top coat?</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1977kok/was_i_supposed_to_use_the_magnetic_wand_before/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>19765m5</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19765m5/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1975xeb</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>My nails in 2023</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1975xeb</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>19752se</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>First time trying blooming gel! 🩵</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqejqhylskcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>197spjw</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Valentine's nails on my shorties</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exsfso361qcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>197r8gb</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>What do you do to save time or speed up stamping?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/197r8gb/what_do_you_do_to_save_time_or_speed_up_stamping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>197px65</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Chrome Nails Look Glittery</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/197px65/chrome_nails_look_glittery/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>197pvmj</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>hanmade press on nails</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197pvmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>197ozda</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>First time using chrome!</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m85twiv16pcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>197miei</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Balletcore Inspired</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oz109jb8nocc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>197m6w0</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Check out my girls work!</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6919s8uzkocc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>197lkn3</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Nail art newbie</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldd045ingocc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>197jxee</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>I absolutely love this work ✨</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197jxee</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>197j55x</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>First attempt at cheetah print… its giving snow leopard but I still love it</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqxyitevzncc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>197i176</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>If you dont know what to get for Vday…</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197i176</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>197d15o</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>These took 7 hours 😮‍💨 worth it tbh, my favorite set ive done.</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197d15o</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>197ajl4</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Gel painted Kuromi on my first gel set. It would've been a better experience if I owned black gel too, not polish. 🫠</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197ajl4</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>197ahk7</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>My Valentine's Day nails</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebgr6epcamcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1975ii5</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>January Nails😊</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92t34hftxkcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jan 17 08:08:17 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_21.xlsx
+++ b/data/2024_01_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C458"/>
+  <dimension ref="A1:C636"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8219,6 +8219,3032 @@
         </is>
       </c>
     </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>198rjd3</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Gold leaf set! By me</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198rjd3</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>198r6s1</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>I got nails that didn’t come with any glue/jel pad thingys</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198r6s1</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>198r5a5</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Soaked off my DIP today. Nails underneath are super beat up, sad and flimsy. Going to try and salvage the growth, with the exception of both my thumbs :(….and start my natural nail journey! Send healthy nail vibes and suggestions my way!</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yax8zm9fycc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>198r4ab</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>I did these myself 🥰</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bj61ud8xeycc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>198qrzi</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Sharp french may be my new fav to do</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198qrzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>198qi4j</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Let's keep it simple</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198qi4j/lets_keep_it_simple/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>198qehl</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Cute nails..check✔️💗</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7akyhbq6ycc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>198n8yu</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Mixed metals ⚜️🪙 inspired by @ gteanails ✨</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198n8yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>198pob6</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Can't get my eyes off my nails.</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3db6hkityxcc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>198pfzd</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>I spent an entire day on these.</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lv1cbbdkwxcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>198p3rj</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Are my cuticles flooded by gel?</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198p3rj</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>198oyrc</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Did my own gel x nails for the first time, how did I do?</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xt3wi04rrxcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>198ovdy</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Can't decided so I got both</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198ovdy/cant_decided_so_i_got_both/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>198op8z</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Leakproof acetone storage</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198op8z/leakproof_acetone_storage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>198k45p</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Watercolor flowers</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198k45p</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>198fu8b</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Got inspired, and had to play around🩷</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxe9912tnvcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>198cnux</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Using nail glue and gel polish on same set</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198cnux/using_nail_glue_and_gel_polish_on_same_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>198bygt</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Static Nails Review</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198bygt</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>198o6ul</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Advice on shape</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198o6ul</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>198bqwa</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Bayou inspired gel nails my sister did! She just started doing nails (slightly grown out lol)</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198bqwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>198ah9r</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>First time using 3D gel for art</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sejbfc8llucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>198nnw4</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>This is the first time I wear such long nails, any advice?</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyqpawk2fxcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>198nd13</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Green cow nails, different lighting different effect.</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198nd13</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>198n5c5</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Manicure?? More like Bi-nicure 😉🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dveqjjcaxcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>198n03k</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Is there any way to slightly change the color?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198n03k</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>198mvvo</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>First time doing gel extensions on myself :)</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198mvvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>198muvs</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Long lasting holographic/cat eye regular polish? Help a girl out</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198muvs/long_lasting_holographiccat_eye_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>198mktn</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>A set of press-ons I did a few months back ☺️ (featuring my cute puppy)</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9p2mrh385xcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>198mgqq</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>How are we feeling about the shape?</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198mgqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>198lz9s</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Making my way through the polishes my hubby got me for Xmas. I quite like this one</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1o21sh10xcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>198lv9f</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Just started doing acrylic!</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcm1l314zwcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>198ldkp</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Mani i did on my boyfriend</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ly4lsy73vwcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>198l4gy</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>I did square nails for the first time and I love them also my first time with the design lol</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jw5ckl0twcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>198kedo</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Freshly painted and feeling fabulous! 💅✨</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/892sd82xmwcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>198k9a1</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>"starry night, city lights.." 🌌</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6g4vegiulwcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>198k3p7</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>January's nails sets 1 and 2</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198k3p7</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>198k2g1</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Questions about Gel</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198k2g1/questions_about_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>198jshu</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>New manicure by myself</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i8robu81iwcc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>198jmfk</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>beautiful in fiery red 💅🔥</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxyncu1mgwcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>198j0py</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Acrylic removal and aftercare</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198j0py/acrylic_removal_and_aftercare/</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>198iruo</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>What’s your favorite nail shape? I use to like long coffin when I was in high school but I think now that I’m older I like short almond. How about you all ?</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urljpyez9wcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>198iecj</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>new full set :)</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198iecj</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>198hznj</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>How do they look?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aybdti3v3wcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>198hlxx</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>winter ❄️ ⛄️</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qowkdsbx0wcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>198hcgp</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>got my nails done literally love them</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p46zw02zyvcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>198h4ra</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>My favorite toes yet!</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6o09jyoexvcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>198gxxc</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Beetles gel dupe</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198gxxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>198gfbc</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Product discussion for ideal manicure.</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198gfbc/product_discussion_for_ideal_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>198g6qu</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>please help me feel better about these 😩</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198g6qu</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>198g307</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Gel nail stickers recommendation</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ux8ijp4mpvcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>198g05m</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>How can I tell the grit on a nail buffer?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198g05m/how_can_i_tell_the_grit_on_a_nail_buffer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>198fad2</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Looking for thoughts/reviews on the Apres beta led lamp to cure gel polish.</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198fad2/looking_for_thoughtsreviews_on_the_apres_beta_led/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>198f3f8</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>My first ever set!</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ylcworjivcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>198f37x</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>I did them myself!!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3krxw1aiivcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>198eydp</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>April 2023 - January 2024</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198eydp</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>198ex0r</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>First attempt at hard gel extensions!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8k7zk5j9hvcc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>198ecce</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Gel nails are peeling off</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198ecce/gel_nails_are_peeling_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>198e8vz</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>New nails by me</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198e8vz</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>198e2e0</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>All that glitters is not gold. Can't wait to try stronger paints that won't chip as easy.</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3yh3o854bvcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>198dthn</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>🥹… i went to a new nail salon..</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4v9hw6f9vcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>198doz8</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>New set for my bday 💖💅🏼</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibbm9npl8vcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>198dc28</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Milky white is way out of my comfort zone</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198dc28</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>198d7kc</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Fresh out of the cabin🦋✨</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2so6gzy45vcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>198d1mj</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>These nails are gone!</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lihp4ftx3vcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>198cyv1</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>my mystical nails, I love them 💖</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7i5yj5g3vcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>198cy52</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>A husband on a mission. I really liked this color combination.</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198cy52</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>198co2e</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>junji ito press ons :3</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198co2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>198cigh</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>A FEW OF MY FAVORITE NAIL SETS I DID IN 2023</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198cigh</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>198cegf</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>I love my new night sky nails! (Done professionally)</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6k56g716zucc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>198bv2b</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Dual Pink Ombré Lipstick Nails🩷</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/volbm5tfvucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>198abf8</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>What does jelly polish look like on top of regular polish?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198abf8/what_does_jelly_polish_look_like_on_top_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>198a56r</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>It’s not much, but I’m happy with my first time doing gel at home!</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7ad5vo7jucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1989zfs</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Lost some length on two, but I won't let it stop me!</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m764gt4iucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1989sp3</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>No professional, but feel better about mistakes.</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1989sp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1989slg</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Cute but simple</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rgfbxtsgucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1989dag</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Filing off gel polish from builder gel</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9lqg8qsducc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>19896sh</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Needed something bright and colorful to get me through this month!</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oyg1wv6kcucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>19894lt</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Winter Cat Eye | Ft: My fav teddy bear hoodie</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1ttmi75cucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>19893dl</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>new nailssss</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4d0kvfiwbucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1988lz7</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Holo Taco's Royal-Tea Blue and Disco Dust Taco was perfect for my cousin's royal blue themed wedding!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oypmc6yg8ucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1987pna</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>How do I get my nails to stop peeling... like an onion??</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19ajvlc72ucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>19885lr</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Recent almond nails</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/759zlrsa5ucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1986vxh</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Uv gel help</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1986vxh/uv_gel_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>19882ow</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>How can I make my nails not look like a 5 year old and hands look like an 80 year old?</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19882ow</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1988129</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Loving my new claws</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1cd0vi4e4ucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1984ilt</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>did something very dumb and now i need advice</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1984ilt/did_something_very_dumb_and_now_i_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1984ieo</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>What kind of nails to get?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1984ieo/what_kind_of_nails_to_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1987uv5</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>My first DIY Gel X Mani!</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9gesrei63ucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1987tw2</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Loving my newest mani - black cherry with a chrome accent (ignore my freezing cold red hands)</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5b6sjpaz2ucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1987rmg</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Faux airbrushed star nails</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n01mtxqd2ucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>197y9px</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Before and after - 2.5 Month growth update</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/197y9px</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>197xtwl</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>*Picture from @nailpom_nico on instagram* Is it possible to achive anything similar with gelpolish? Thanks!</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sk3x5nq8grcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1986hv8</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wateeeer nails </t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pdzyl5icttcc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1985v23</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>New nail day cause my nails grow real fast with acrylics</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9z1buppotcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1985s2f</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Ohora Nails</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1985s2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1985o5l</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Please Help! Will the Cold Ruin My Nail Products?</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1985o5l/please_help_will_the_cold_ruin_my_nail_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1984qvp</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Just finished these, wanted to share 🥰</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/mvLE8WN.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1983xlx</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>I'm proud of the nails I did for a client.</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vo5pdaxj9tcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>19839bj</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>I love this! Acrylic press ons!</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yjn81ulw3tcc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1982pom</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>🥲 should I chop em all, or just get an extension on our fallen comrade? Any shape reccomendations?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvjmgpxuyscc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>198ptoo</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Don't use coconut oil as a moisturizer after a pedicure </t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7fqf7gjf0ycc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>198oqme</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Questions for Hella Handmade buyers</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198oqme/questions_for_hella_handmade_buyers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>198iv45</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>I have bad nails someone know how to get them long. respont please</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198iv45/i_have_bad_nails_someone_know_how_to_get_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>198i28m</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Semi cured gel nails</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198i28m/semi_cured_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>198hu6w</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Builder Gel or Rubber Base for reg polish</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198hu6w/builder_gel_or_rubber_base_for_reg_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>198obb6</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>ILNP is smudging!</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198obb6/ilnp_is_smudging/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>198o9n9</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Couldn’t pick between velvet and cat eye…so I did both</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1lhpn8stkxcc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>198nlo6</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Love how ethereal these turned out!</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198nlo6</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>198nasi</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Shaped Magnetisation Galore</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198nasi</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>198morc</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Mourning 😞</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqurgrn66xcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>198m9s8</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Beetljuice Beetlejuice Beetlejuice</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onbsr9vd2xcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>198m7bk</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>UP vs Aurora</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198m7bk</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>198ldop</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Favorite nudes for dark skin?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198ldop/favorite_nudes_for_dark_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>198l38k</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Out the Door QDTC lifts color off</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198l38k/out_the_door_qdtc_lifts_color_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>198kykk</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>ILNP Misty</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198kykk</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>198kfbq</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Base coat question.</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198kfbq/base_coat_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>198kcyf</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>"starry night, city lights.." 🌌</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6irabdgpmwcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>198k3jx</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>You ever just do your nails and then get bored 2 days later then add a topper to try and keep your interest?</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198k3jx</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>198k0bu</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>How can i achieve both these looks?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198k0bu</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>198jrp6</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Cheap peel off base</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198jrp6/cheap_peel_off_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>198jicm</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Emerald jelly with pink/orange shimmer 🌸🍊</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198jicm</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>198j73n</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Dreamscape</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198j73n</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>198iqim</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Burning Coals</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198iqim</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>198hzyn</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Unicorn Pee vs Aurora Pigment?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198hzyn/unicorn_pee_vs_aurora_pigment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>198hnko</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Tried heart magnetics again w/ 4 new colors!</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198hnko</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>198ga07</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>It's a crummy paint job but I've wanted this color for so long!</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198ga07</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>198fz95</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Had to play around, while I was inspired🩷🎀</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198fz95</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>198ff89</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Orly - Coffee Break ☕</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198ff89</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>198faty</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Does Anybody know a good substitute for Brucci Moonshine (423)</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198faty</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>198eztz</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>🖤Geometric Gradient🤍</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198eztz</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>198eusz</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Color shifting Neko(s)</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198eusz</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>198e73p</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>I don't known how this color can get any negative feedback</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198e73p</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>198e52l</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Happy with Glowing Mushroom ✨🍄✨</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3uozvqnbvcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>198e41n</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>The neodymium bar magnet from ppu doesn't mess around</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198e41n</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>198dknv</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Mooncat Magnetic ❤️</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198dknv</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>198cw0u</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Magical 💙💚</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m0pa2res2vcc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>198cogw</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Zoya 'ono'</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fng1m5pd1vcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>198cetd</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Cirque Tahitian Pearl</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198cetd</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>198c89p</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>First time ILNP</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wxra2v4yucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>198bxvl</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Mooncat Millenia</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198bxvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>198audl</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Hygge</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/douclt94oucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>198atdn</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Brrrr 🥶</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198atdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>198afda</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Feelin' Frosty!</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198afda</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>19895ua</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Holotaco versus Mooncat Base/top coats?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19895ua/holotaco_versus_mooncat_basetop_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1988xlo</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Mermaid Bait working extra hard today</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4vzr39raucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1988q12</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Glitter polygel, what color or design should I do on top?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8zascn99ucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1988knk</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Inspired by the garnet girls, gold-dipped gradient!</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1988knk</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>19886sw</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Flourish on periwinkle/lavender</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19886sw</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1987usa</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>An all-time favorite 💙</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpsdx3z53ucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1987b6v</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Cute or bruise-like?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1987b6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>19876r3</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Needed a little sunshine since we've been having a horrible cold snap</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19876r3</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>198709z</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>KBShimmer How Polarizing</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198709z</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1986o37</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>finally some sun today to take a proper photo 💅</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26rvzcmnutcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>198642k</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Holy Faded polish Batman!</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198642k</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1985puh</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Took my time with application - OPI My Solar Clock is Ticking</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/QOUXLlE.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1985ow0</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>question about base coat/stickers</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6jyw0wentcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1985gdm</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>{PR} The Drama Queen Quartet (My Collab!!) 🥰</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1985gdm</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>19857fb</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Help me pick a thumb design?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9m7dfzesjtcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1983wsz</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Mooncat Outlaw Country</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4la23oi9tcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1983ked</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Gentle/health for nail manicure?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1983ked/gentlehealth_for_nail_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1983hdj</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Not my best..</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1983hdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1983f4h</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Lunar New Year nails</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rq53cytd5tcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>19835u0</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Subtle Snowflake Nails</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19835u0</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>19835ax</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>matcha made in heaven 💚</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19835ax</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1983258</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Newfound love for Eclipse</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sjid0pm42tcc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>198156q</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>I might have gone slightly overboard trying to dupe Vaporize</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198156q</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>19809fw</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Trying to find nail polish that matches my lipsticks, but it's tougher than I thought. Please, help me♥️</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19809fw</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>197z77h</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Nude alternatives for brown skin?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1touau2dxrcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>198m8n5</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Last night I discovered my ring finger glows in the dark!</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198m8n5</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>198m2rt</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Love?💜</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ufd8avw0xcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>198jt6l</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Proud of my DIY nail art!</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198jt6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>198jjwd</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>I love how the “cat eye/velvet” nails have come back into popularity. These two are my favorite I’ve done recently!</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8n9rxsw2gwcc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>198gxfo</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>When you ask a guy for nail inspo and they bring up their favorite video game 🥲</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3kavedvvvcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>198f737</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>i did nail art of some flags</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s21npxc9jvcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>198a048</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Lost some length on two, but I won't let it stop me!</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8m72w6q9iucc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1983yxx</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>I'm proud of the nails I did for a client.</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0a94z4x9tcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1983jqf</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>I do love the snow 💙</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpsr3nhg6tcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1981j4f</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Id take all shades of purple 🤑</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1981j4f</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jan 18 08:08:03 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_21.xlsx
+++ b/data/2024_01_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C636"/>
+  <dimension ref="A1:C798"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11245,6 +11245,2760 @@
         </is>
       </c>
     </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>199kud2</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Cat Eye ft. Airbrush</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0xjxli8kl5dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>199kyf7</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>First time trying a gradient</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199kyf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>199kxps</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>how can i(14F) grow stronger nails?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/199kxps/how_can_i14f_grow_stronger_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>199kcxm</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Shape of press-ons ok?</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199kcxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>199kfop</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>new set 🎀</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199kfop</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>199k8ff</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Continuously clipping uv gel nails...</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/199k8ff/continuously_clipping_uv_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>199ioek</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>done on me by me</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7myyajadx4dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>199hqf6</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Im obsessed with reflective glitter</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95adoeg6o4dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>199hz4m</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>subtle valentine’s day themed nails!</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1tahpcjq4dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>199hxdy</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>are these almond or oval?</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199hxdy</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>199hx9i</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>My dad said these looked like alien veins haha</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5lku3l0q4dc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>199hhwr</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Pink Chrome Birthday Nails 🎂</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcrsmh7vl4dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>199eypm</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Advice for short nail beds and damage</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199eypm</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>199e2xz</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Gap with Press Ons</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyt15hopr3dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>199gfjq</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Good strengthener?</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/199gfjq/good_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1998xwz</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Is gel actually bad for your nails?</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1998xwz/is_gel_actually_bad_for_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1998emj</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Can anyone tell me what brand/color dip powder this is?</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1998emj</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>199etsc</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Ready for my cruise</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6dzwtbgwx3dc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>199e7nm</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Some of my favorite sets!</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199e7nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>199dcpb</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>First time doing gel nails, advice?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bctnlq7kl3dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>199cuqj</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Fresh set 🌿💅</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvzpakneh3dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>199cqha</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Painting with my left hand 🫠</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qla77o9fg3dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>199cl83</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>hello kitty strawberry nails i made last night 🍓 in love with them ❣️</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jt7tux2bf3dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>199bq53</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>I call it, “elegant calico” 🐱</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nk2od25q83dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>199al8k</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Gel method dip question</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/199al8k/gel_method_dip_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>199aklz</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>second ever set i’ve done myself!</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eth1xxqsz2dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>199akfn</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>I’ve been really into browsing Japanese Nail Art IG recently— been trying to emulate them</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199akfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>199a6ui</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>I hate my nails</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hmseav1yw2dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>199a2wj</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Winter Nails ❄️</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g33tq4i4w2dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1998v4v</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Any tips on how to stop biting and destroying my nails ? How to grow them faster ?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxdxf4p6n2dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1998pd6</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Peachy French Tips! 🍑</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1998pd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1998et6</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Extra short coffin? I think I love it</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1998et6</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>19982k8</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Tipping norm?</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19982k8/tipping_norm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1997n25</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>question</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6sut04gce2dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1997dht</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Short(er) red french mani</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0d7bzsic2dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1997ai7</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>First set of 2024</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8k4465yb2dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1995wyj</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Did my own nails! Thoughts?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6vm01v722dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1995t3w</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>First set of 2024</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blpkbwfu02dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1995fmh</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>could i do a simple gel fill in at home?</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ey1czmuy1dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1995bl7</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>beautiful and delicate nails</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vluyoje1y1dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1992xu2</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>what can i add to make these better ?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4xbpq67h1dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1992ba6</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Why do my nails have different colors?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1992ba6</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1993wiz</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Silk wraps</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1993wiz/silk_wraps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1993pg6</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Coming up on my 3 year anniversary of being cancer free! I continue to grow. (White and burgundy are the colors for head and neck cancers)</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mb67qfuul1dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1993mno</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>(old) new year’s eve nails :p</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fuqbmn1m1dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1992i81</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Day 13</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1992i81</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>198u7o3</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Thoughts on this apex?</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198u7o3</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>198pb00</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>3/09/23 when I stopped using press on nails - 13/01/24 my nails now after finally trying to care for them!</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198pb00</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1991t6c</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Barbie nails 💅🏼🎀</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ul8ug2hh91dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1991evg</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Looking for better adherence</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1991evg/looking_for_better_adherence/</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1991e7f</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>i’m in love with this colour</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8wlvj9t61dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>19912jo</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Made these press ons and I'm in love &lt;3</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19912jo</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>19910ia</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>My nails a day before they broke</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2opnn6o541dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1990tvd</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>First time doing my nails. Tips?</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1990tvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1990fad</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Free hand French tips 😊</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1990fad</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>198zsvn</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>cherry nails🍒✨</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198zsvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>198zglg</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Ombre French with clear chrome on top</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198zglg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>198z50s</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqr13b4tq0dc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>198z0i0</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>First attempt at GelX</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3vs2ijup0dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>198p7ck</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Purple early valentines nails inspired by Belle Beauty on pintrest 💜</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198p7ck</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>198su3d</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Can someone please explain to me what are gel nails and what are acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198su3d/can_someone_please_explain_to_me_what_are_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>198w9ng</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>I forgot to post my nails I got done for New Years! These were night court inspired! From ACOTAR. ❤️🔥 they have grown out since .... new nails getting done today!</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9ksvjky20dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>198y5k2</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>How to fix cuticle stains?</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4i47378j0dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>198xryb</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>My early Valentine nails</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oy0ker73g0dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>198xorl</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>So obsessed with this acrylic color</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lpcg4ecf0dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>198xh2g</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>How much of your nail can you actually repair?</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198xh2g/how_much_of_your_nail_can_you_actually_repair/</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>198xau2</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>First 2024 nails! And advice needed!</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198xau2</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>198wrpm</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>My first 2024 nails 😃</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lma01rrj70dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>198wqqx</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Advice</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3tvmqxa70dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>198wojt</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Sometimes a simple gel overlay just fire🔥 I’m loving understated nail designs rn ✨</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yevajtq60dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>198wlid</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Just got them done today</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198wlid</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>198w7w3</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Valentines nails❤️</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/af0ikvch20dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>198vy5p</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>very shiny new nails for me</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bpwufzyzzcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>198vaef</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Went to a new nail tech and was not disappointed!</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufz39t9btzcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>198v1ds</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Glisten and Glow - Time Together</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198v1ds</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>198uy11</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Please how did i do on these set. any advice</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9i3labxepzcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>198toiq</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>What colours/designs would look well in very short nails (almost no free edge)?</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198toiq/what_coloursdesigns_would_look_well_in_very_short/</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>198tljg</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Redid my nails. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198tljg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>198thhl</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Good nail shop?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/198thhl/good_nail_shop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>198sqh0</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Blue blue jeans. 💙</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ijtf0skzycc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>198spnu</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>I love my new nails!</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emebv17azycc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>198s0rj</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Is my nail broken?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198s0rj</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>198rvqw</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>My January nails!</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zv44jnveoycc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>198rtez</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>biab frenchies 🩷</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ro5oydgpnycc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>199ks7j</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vortexing a magnetic polish </t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bdugp9ttk5dc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>199kp6r</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Mooncat &amp; Starrily</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8k20ofasj5dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>199kna4</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Anyone know a good dupe for this Ruth Polish?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199kna4</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>199kkfs</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Relearning nails, but haven't tackled the subject of cuticles and proximal Folds yet. I experience mine being very rounded while Press-Ons/Lazy Girl I like often are square (as demonstrated in color). Sometimes I file to fit, but curious if caring for cuticle will square it up a bit?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cewhvuh8i5dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>199jsxk</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>My second at home gel mani!</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199jsxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>199jh3b</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Essie Shade Similar to This?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuqsj4qn55dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>199jchk</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>favorite nail combo</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6boem7a45dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>199i0ux</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>First Time Ordering fron ILNP - Any Must Haves?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/199i0ux/first_time_ordering_fron_ilnp_any_must_haves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>199hmgf</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>My husband said my shirt was green...</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199hmgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>199hgyb</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>what polishes to get this look?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hr7743ml4dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>199h1p1</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>That Zoya sale paid off</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199h1p1</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>199gzqe</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Is it just me</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199gzqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>199g1rq</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Do I need to worry about pushing my cuticles too far back?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3p9s4ck84dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>199g0dk</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Mermaid bait</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57qdk2j884dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>199fxy5</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Enjoying my naked natural nails right now!</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/soc2r3an74dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>199fsii</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>workshopping a Valentine's Day mani (and my first skittle, AND my first time using Seche Vite!)</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199fsii</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>199fs47</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>E file on gel</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/199fs47/e_file_on_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>199fqso</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Clear coat +colour over shellac</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/199fqso/clear_coat_colour_over_shellac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>199fcny</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Honestly becoming more and more proud of my ability to do my nails at home!</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9g8agkdk24dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>199eo56</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Please help me solve the mystery of the polish that doesn't exist (except it definitely does because I own a bottle)</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/199eo56/please_help_me_solve_the_mystery_of_the_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>199ekvu</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Savagely bitten</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199ekvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>199ct3x</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Ethereal shipping times?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/199ct3x/ethereal_shipping_times/</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>199cnrg</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Advice on a manicure</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/199cnrg/advice_on_a_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>199cgo8</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>was eating froyo and noticed i’m matching my spoon</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199cgo8</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>199ccjk</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Rainbow Blues</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fe4f8hhd3dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>199bb5m</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Mauve Marble Madness!</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zr3anqe53dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>199bb1h</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Winter Blues ❄️</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199bb1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>199a1cs</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Is there a way to replicate this texture without gel polish?</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/199a1cs/is_there_a_way_to_replicate_this_texture_without/</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1999yy5</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>First set of gel X Extensions I’ve ever done 🥹🤍</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1999yy5</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1999x5m</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Reclaim the Flame - Mooncat - velvetized</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yijuj4zvu2dc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1999pvl</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Cirque Colors New Good Vibrations collection</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://youtu.be/TLhfkVpU5dc?si=qL6NWNttIcY6QYNu</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1999ob9</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>LPT: smudged polish? steam it back!</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gd9qqea4t2dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1999e7d</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>yeah, fairy dust lives up to the hype</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1999e7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>19992gr</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Just my nails unintentionally matching my jacket</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19992gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>19985rj</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>KBShimmer Sunset in My Ways</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19985rj</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1998387</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Holo Taco "Nightshade" &amp; "Freezer Burn"</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3574yvkh2dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>19978j7</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Nail polishes that strengthen nails?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19978j7/nail_polishes_that_strengthen_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>19971n9</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Scuffed topcoat</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19971n9/scuffed_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1996hdx</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Why is my polish “breaking?”</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1996hdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>19962eh</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Mooncat Mermaid Bait</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cm0r8bb32dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1995u78</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Remove Gel-X Press Ons</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1995u78/remove_gelx_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1994sgs</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Me trying to convince myself that the polish is the same as the swatch pics</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jw11kmdau1dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1994niu</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Montego Bay</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1994niu</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1994f7v</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>💎💜Amethyst Geode💜💎</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1994f7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1994ctq</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Thinking of starting gel nails but I don’t want to buff</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1994ctq/thinking_of_starting_gel_nails_but_i_dont_want_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1994bwx</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Nail polish dupe for these?</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uro2hoe0r1dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1994bjf</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Any other rock climbing lacqueristas?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1994bjf/any_other_rock_climbing_lacqueristas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>19948b1</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>1 coat blue and admirable restraint 😌</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/pd46cnU</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1993pmr</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Zero Degrees with snow and sun!</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4hs55rhmm1dc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>19931je</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Soft spring in winter nails!~</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19931je</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1992xnn</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>I knew I kept this piece of ledge for a reason! I just didn’t think it would be for a photo shoot with my new nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1992xnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>198xz1j</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>💙🦋 Polished Used: Picture Polish (Shade: Alice) | Seche Vite (Gel Effect Top Coat)</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198xz1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>198xh7g</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Nothing like a bright coral in January! Polishes Used: Zoya (Shade: Journey) | Seche Vite (Gel Effect Top Coat)</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198xh7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1992kge</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>ILNP Zero Degrees ❄️🧲</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qn0vatyne1dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1992i6k</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Miss Chanandler Bong 💜🩷🩶🩵</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28a2ip18e1dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1992hw7</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Gel manicure by me 🥰</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1dkgp6u4e1dc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1991aqc</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>O-B-S-E-S-S-E-D with this Bluebird Polish</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1991aqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>19909lt</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Phoenix: Girl Dragon</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44pwpha1z0dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>199031c</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>DVN - Joshua Tree</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199031c</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>198zkey</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Sin Eater</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198zkey</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>198zffu</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Looking for a polish shade</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198zffu/looking_for_a_polish_shade/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>198xijt</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>A dupe for this shade?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198xijt</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>198xhyw</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Prep</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198xhyw/dazzle_dry_prep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>198x1r3</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Your experience with KBShimmer Fillin' Groovy base?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198x1r3/your_experience_with_kbshimmer_fillin_groovy_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>198vr47</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Which pedicure color should I go with? I’m trying to choose between Sally Hansen ASAP Apple (classic red) or Essie Bahama Mama (deep plum)</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/198vr47/which_pedicure_color_should_i_go_with_im_trying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>198v6kp</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>ILNP VIP, didn't get the hang of magnetic effects yet, it's quite dispersed</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198v6kp</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>198uy1t</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Glisten and Glow - Time Together</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198uy1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>198u2dd</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>How often should I be bring my nails done - question on growth &amp; greenies!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198u2dd</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>198scrn</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Hello kitty!</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198scrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>199hf9x</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>❤️</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1j0l876l4dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>199dme7</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Molding gel flowers!</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0a0doadsn3dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>199cmkj</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>strawberry picking with kitty! 🍓❣️</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199cmkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1998yyx</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Iridescent powders really are magical. Before &gt;&gt; After</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1998yyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1993s2y</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Practicing reverse stamping</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76ej8f74n1dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1993dk4</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Ill never get tired of Strawberry nails</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9n9n5v9k1dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1992w36</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>It themed nails</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r32rnyfxg1dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>198xm5q</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>3de gel x set since transitioning from doing dip powder</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0l2b0ujqe0dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>198u0k0</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Thank you nail stickers</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/198u0k0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jan 19 08:08:20 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_21.xlsx
+++ b/data/2024_01_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C798"/>
+  <dimension ref="A1:C962"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13999,6 +13999,2794 @@
         </is>
       </c>
     </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>19a05j4</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>what shape would suit me? :’)</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a05j4</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>199z9h4</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>At home diy-er. Gel extensions never stay on my right hand</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/199z9h4/at_home_diyer_gel_extensions_never_stay_on_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>199yoe4</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Injured cuticle on gel nail, shall I remove?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/199yoe4/injured_cuticle_on_gel_nail_shall_i_remove/</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>199zs6c</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>I was so nervous to attempt this but I think I did amazing for my first time doing something like this!</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/11tw2xjec9dc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>19a2edc</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Nail care</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a2edc</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>19a3kzq</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>I’ve burnt my nails with UV light a few times now, how can I prevent this from happening again?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19a3kzq/ive_burnt_my_nails_with_uv_light_a_few_times_now/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>19a4hkk</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Newbie Question</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19a4hkk/newbie_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>19a4ty7</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Nail care/help</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a4ty7</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>19a91pl</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>New nail art! inspo from nuocmamkimchi- ur nail art was so cute 🫶🫶</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a91pl</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>19ab03n</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Should I do a moon and stars or keep them plain? Im torn. Or other design ideas?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h7qkf05pvbdc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>19ab1ri</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>getting my nails done for the first time</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ab1ri</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>19adckm</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Latest practice set, my thumb started chipping at the corners :(</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19adckm</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>19ad9ck</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>I love this set so much. Took me hours to design and make it</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m204c01kjcdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>19ad065</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>What do you think about my next nail target?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2go8szfgcdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>19aczlx</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aczlx</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>19a70rf</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>I didn’t take off my gelx nails properly and now my nails and damaged/bendy</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19a70rf/i_didnt_take_off_my_gelx_nails_properly_and_now/</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>19a78me</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>The best “what I showed nail tech vs what I got”</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a78me</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>19a98x4</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>What's wrong with my nails (gel on natural nails)</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a98x4</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>19aas62</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>good nail glue to not damage nails?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19aas62/good_nail_glue_to_not_damage_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>19acpp3</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Black glitter gel over natural nails</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1t8xzs7dcdc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>19acc0q</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>I need to learn how to take better pictures 😅</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfr4qqp39cdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>19ac8dh</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Latest fill :)</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6mvy8jz7cdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>19aap3r</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Homecoming Nails</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7wc76qpsbdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>19aaa91</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Gel Manicure</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4n0kzmmobdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>19aa8cq</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Simple cat eye v-day nails!</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aa8cq</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>19a9f2g</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Love iridescents</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnouh7kigbdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>19a8vak</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>went a bit more simple this time</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zoktj6qbbdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>19a8efj</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Efile on natural nails advice</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ochq26yn7bdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>19a89ug</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>My mini nail polish haul</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xan87jwh6bdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>19a7xw7</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>I dont love how these came out</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22pa048k3bdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>19a7uuj</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Did several different styles to celebrate my sisters birthdays!</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4u9uhmmt2bdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>19a7isb</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>My crow brain is obsessed 🥹💜</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a7isb</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>19a78pz</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Got cat eye nails for the first time:)</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4r9pps2lxadc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>19a73rs</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>☯️</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cibph2agwadc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>19a710j</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>First set of the year</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3be9j6gsvadc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>19a6jr4</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>I am OBSESSED! Blue, purple and silver chrome.</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lmzx21rradc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>19a5iz2</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>I love them</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a5iz2</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>19a5dhv</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Please help</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a5dhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>19a4t47</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>My first set of the year, zebra 🦓and electric blue 💙 on natural nails (hard gel) 💅 by @tank__nails on IG</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a4t47</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>19a4sff</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Finally did black for the first time 😍</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8a2h52gdadc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>19a4s4w</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>best manicure ive ever had</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56u4epxddadc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>19a4r8m</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>New sheer pink dip set!</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a4r8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>19a4ld6</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>First time getting gel x, love how they look 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a4ld6</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>19a4ahy</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Lace ✨</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucoa4enj9adc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>19a3gjq</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Opals and pearls ✨</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a3gjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>19a3db1</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Business in the front... party in the back?!</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a3db1</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>19a2tmb</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>🎀 hello kitty + gel x🍦🌷🍒</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhezn0fjy9dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>19a2rnn</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>I love my new nails! although it took me 2 hours to type this! lol.</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kd25ydgmx9dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>19a2qsj</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Best 3D sculpting gel?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19a2qsj/best_3d_sculpting_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>19a24n8</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Remember when OPI had matching lipsticks?</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dge833et9dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>19a1tfn</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>He got so many things right, then he added the wrong glittery effect. Yet I’m obsessed with the rest</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgovrxq3r9dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>19a1q1m</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Can I use a rubber base and add builder gel</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19a1q1m/can_i_use_a_rubber_base_and_add_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>19a1lt3</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Is it too early for valentines sets 🤭</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a1lt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>19a1jix</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Handpainted valentines looney tunes nails 💅tutorial on my tiktok @thenailpalette23 😍</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xo89t532p9dc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>19a1dgu</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Nail advice- why isn’t my gel curing?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a1dgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>19a1c5t</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>🔮💫</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a1c5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>19a12nq</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>💎💜Amethyst Geode💜💎</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a12nq</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>19a0mzq</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>New Year, new nails ✨</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4h0nfkmi9dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>199yo1p</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Vampy red.</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dw9puh7b49dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>199ylup</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>for pink fans like me</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l23xd6ov39dc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>199y4e1</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>hello. I wanted to show you this frech glaze design that they did for me at a nail salon. I loved them</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zi14yakb09dc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>199y1m0</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Do you mind quiet clients? I am wondering if I am weird..</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/199y1m0/do_you_mind_quiet_clients_i_am_wondering_if_i_am/</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>199xn9z</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>using liquid chrome products with regular (non-gel) lacquer?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/199xn9z/using_liquid_chrome_products_with_regular_nongel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>199xkw7</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Just want to show how talented my nail tech is!</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199xkw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>199x664</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Builder gel apex flattens out and floods my cuticles while curing in the lamp</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/199x664/builder_gel_apex_flattens_out_and_floods_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>199wtr0</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Icy chrome cause winter isn't over yet</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199wtr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>199wsea</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>new set 💅🏽</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z037seulq8dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>199wilw</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>are you able to make acrylics pointier after applying nail polish?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/199wilw/are_you_able_to_make_acrylics_pointier_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>199whs4</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>my nails said rawr in the last pic</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199whs4</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>199wdcv</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Help? (Need advice)</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199wdcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>199w24p</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>One of my favorite sets 😍</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4as6nqal8dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>199w0g7</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Unintentionally matched my lunch</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k34a6xuyk8dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>199vp5f</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Evangelion Nails💜💚🖤</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9q9tg5oi8dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>199vnzm</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Will making a biotin paste help nurture nails?</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/199vnzm/will_making_a_biotin_paste_help_nurture_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>199uydq</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Need help making press on nails not feel rubbery</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20c07o62d8dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>199uxcq</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Pink stiletto nails!</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7azvx7quc8dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>199uws1</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Still new to doing my own - how are my Valentine’s Day nails???</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkwt2ufrc8dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>199ul8w</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>🎀</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ll3plvfa8dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>199u1a8</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>I‘m in love with my new nails! What do you think?✨💗</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7o9zb0gb68dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>199tnf7</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Do you like dreamy chrome? My nail broke so I came back for revenge with this one! (◍´ᯅ `◍) 💗</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199tnf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>199tk01</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>🧡Holo Taco Tax Haven 🧡</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199tk01</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>199t6jj</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>guy here. finally got around to white 🤍 Gel-effect ☺️ Done myself 😉</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/01glthhpz7dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>199sqnq</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Me-Ow 💕</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199sqnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>199snqv</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Subreddit for doing your own nails at home?</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/199snqv/subreddit_for_doing_your_own_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>199sh3d</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Early Valentine Set</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ahol6z5u7dc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>199r93h</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>A little early for Valentine’s Day, but here we are. 🥰💌</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwzcqes3k7dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>199qp7k</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Blue &amp; Silver 💙</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3x19vcvff7dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>199pc08</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>My current press-ons remind me of fossil rocks.</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199pc08</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>199onbr</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Older set</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnvgrlvhv6dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>199nw6a</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wj3gd1mbn6dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>199mlf8</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Pretty in pink?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0kwzgvx76dc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>199miqh</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>My tech is amazing! The last set I got:)</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4f91i27w66dc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>19ad5ip</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Anyone they Nailpollies?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53kakofbicdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>199xjhk</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Can't stop looking at my Super Shifty nails</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199xjhk</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>19ab55e</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sometimes all I want is glitter </t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hhs5m271xbdc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>19aaskl</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Honesty</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1vowb1otbdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>19aakaa</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>This might be a silly question, but is it safe to paint the underside of your nails?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1io5kecrbdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>19aa21c</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>The perfect pinky neutral 💖 one coat OPI Put It In Neutral and one coat Baby Take A Vow</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fohr1p4imbdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>19a9wn0</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>G&amp;G Combo💙</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a9wn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>19a8t04</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>I call it Carnival Glass</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a8t04</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>19a8stf</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Zilla+ subscription</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19a8stf/zilla_subscription/</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>19a8f7x</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Blue 💙💙💙</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/owmmch5u7bdc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>19a8a23</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Love this green gold! Essie high voltage vinyl.</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g81ism1k6bdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>19a7qe6</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>I broke a nail beyond and had to change nail shape or chop. Chose to shape but, does this look ok? It feels weird.</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a7qe6</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>19a5xi0</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>At least it's a start. My first home manicure after a terrible experience at a salon.</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahx61puimadc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>19a4xm0</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Proud of my nails ❤️🎉 it’s my first time doing a look this creative in years!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a4xm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>19a4qga</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Zoya Sale + Shipping Fauxpas</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19a4qga/zoya_sale_shipping_fauxpas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>19a4lym</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Vintage by Olive &amp; June but lighter?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2m3zs3l0cadc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>19a4hrx</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Dragon Scales and Tectonic Shift</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a4hrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>19a4hik</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Like little opals on my fingertips</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a4hik</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>19a4ga0</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Replacement brushes for ILNP?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19a4ga0/replacement_brushes_for_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>19a44nz</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Change of plants</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9qtbu59a8adc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>19a3513</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Painted Polish - Star Struck</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a3513</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>19a2yvy</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Finally tried all my Christmas polishes</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a2yvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>19a2763</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Will this also work with ILNP's magnetic (regular) nail polish?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a2763</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>19a2391</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>My mini nail polish haul!</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkm2e5q3t9dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>19a1rfn</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Rubber Gel Removal Help</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19a1rfn/rubber_gel_removal_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>19a0vc2</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Question about chipped ends</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a0vc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>19a0mzf</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>My nails kinda match my soda! 🌼🥤</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gxw1ljmi9dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>19a08vk</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>{PR} Too cold for thermals 🥶</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7bvdvnsf9dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>19a014c</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Anyone can tell me how this effect was made?</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a014c</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>199zgnk</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Sassy Saints nail kit</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/199zgnk/sassy_saints_nail_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>199z2io</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Mani for the deep freeze ❄️ 🩵</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5hwwrt779dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>199yz20</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Customer Service Experience - Zoya</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199yz20</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>199ywin</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Does anyone have reccomendations for a long wear nude polish to achieve the french tip look?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/199ywin/does_anyone_have_reccomendations_for_a_long_wear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>199y6b6</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>another blue january manicure checking in for role call 🫡☃️</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199y6b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>199x435</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Cuticle question!</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/199x435/cuticle_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>199x3nw</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>It’s bluetiful</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199x3nw</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>199vwwt</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Tried something more creative 💚</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h431iz28k8dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>199vuel</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Boring, yet beautiful ☺️</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nuoxwpcqj8dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>199umaj</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Brush question</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/199umaj/brush_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>199tsh1</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>me every time i decide that the perfect time to redo my nails is right after a big ol' cup of coffee</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1yo77de948dc1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>199thv4</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Holo Taco Tax Haven 🧡</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199thv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>199sojl</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Toppers are enhanced reality</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199sojl</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>199sb7a</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>New pedicure color</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199sb7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>199r5ji</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Flower nail art 🌸</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199r5ji</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>199r42n</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>One year of DIY progress!</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199r42n</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>199qoid</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Blue &amp; Silver ❄️</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxkvgzg9f7dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>199q0oh</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>I have accepted the cold and went for a winter themed match. Lumen - Sugared Plum on my left hand, Fancy Gloss - Utopia on my right.</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199q0oh</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>199pvpx</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>ISO Cirque Color Polishes</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199pvpx</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>199pk1k</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Nail polish chipping off edges</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199pk1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>199pa57</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Bat Bitch Dupe?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/duaf0umz17dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>199p7vo</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Paperclip heart with regular magnetic polish</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8kv1obsc17dc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>199oj11</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Older set.</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzvrvf4cu6dc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>199mebo</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Does "don't flood the cuticles" count for base coat?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/199mebo/does_dont_flood_the_cuticles_count_for_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>19aa8o1</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Simple cat eye v-day nails!</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aa8o1</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>19a9n24</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Starfield</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whrnljzmibdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>19a9cqa</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Matching Set.</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5ynyi6zfbdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>19a4x3f</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>My first set of the year, zebra 🦓and electric blue 💙 on natural nails (hard gel) 💅 by @tank__nails on IG</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19a4x3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>19a3nhf</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>took me one day to finish this</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzrxlxwj4adc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>19a395h</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>My nails and their new wine-glass look. Love them.</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b37zrmye1adc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>19a1hd9</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Handpainted looney tunes valentine's nails 💅🏾 Tutorial on my tiktok @thenailpaletteuk</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cka5pjzlo9dc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>19a139f</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>my new set, all hand painted by me, butterflies and flowers are my favorites!</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ienw0jzpl9dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>19a0ftf</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>3 out of 5 of my Barbie and the Diamond Castle nail art ♡</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/179j5ef6h9dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>199ztcb</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>First time doing something like this! I love them !</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oiub970nc9dc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>199z74t</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Not perfect, but im definitely going to practice this more!!</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8j1im46789dc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>199y146</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Valentines set I made recently. Took FOREVER but I feel like I’m getting a lot better with my art 🥰</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkfuuwvmz8dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>199xlcp</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Happy Anniversary to my Trek Nails!</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncbg0qhaw8dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>199vmb1</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Playing around with chrome powder to get a textured gold look. Didn't work with the fellow on the left but I like the other ones</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvjfympmh8dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>199ux6f</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>🌈Rainbow ombré with iridescent glitter✨</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199ux6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>199u6ca</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Does everyone like this kind of watercolor design?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l76ors5c78dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>199tztm</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>What do you think of my nails?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3w00y7x068dc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>199sryo</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Me-Ow 💕</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/199sryo</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>199qh56</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>🖤</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zgg82xdd7dc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jan 20 08:07:26 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_21.xlsx
+++ b/data/2024_01_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C962"/>
+  <dimension ref="A1:C1135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16787,6 +16787,2947 @@
         </is>
       </c>
     </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>19b6dlx</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Russian Navy - I love it!</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0k4hfeusjdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>19b68ho</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>TikTok · mysticmanis</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/t/ZT8puDsjt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>19b62pa</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Simple silver x pink set / Chinese New year set</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19b62pa</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>19b5x2p</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Would this offend a nail tech?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19b5x2p/would_this_offend_a_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>19b5kd9</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Coquette style. I'm ready for valentine's day 💘</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3s5p9ahjjdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>19b5exx</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Best LED lamp?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19b5exx/best_led_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>19b51c7</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>How to make them look better 🥹</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19b51c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>19b4w47</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Should I take these off? It’s been about a month and I am not sure if they are too grown out yet or not.</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meo21kv5cjdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>19b4jld</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Putting acrylic on rubber base gel?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19b4jld/putting_acrylic_on_rubber_base_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>19b3s6j</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>HELP!! Does any brand make a clear red acrylic nail powder?</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19b3s6j/help_does_any_brand_make_a_clear_red_acrylic_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>19b3jz1</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Press on nails from etsy</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19b3jz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>19b3hnq</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>rubber base gel or builder gel in a bottle?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19b3hnq/rubber_base_gel_or_builder_gel_in_a_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>19b2tts</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Café ☕️ swirl</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29rwsy51ridc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>19b2hh6</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Butterfly set</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/md8kp31snidc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>19b2551</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Tried out a new gel x set</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19b2551</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>19b1wr0</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Loving this bright orange this winter!</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzleg9vdiidc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>19b1oj3</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Close up of this BIAB mani from yesterday 🍬</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klr45kfbgidc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>19b1kly</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Birthday Nails ♒</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19b1kly</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>19b1cwr</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Regular Polish + gel?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19b1cwr/regular_polish_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>19b1a41</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>had to cut my nails short for work 🫣 are these nubs still semi-cute at least?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19b1a41</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>19b17fa</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Simple Sparkle</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19b17fa</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>19b1176</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>can't wait for love season, inlove with my nails🥰</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hmd36qy9idc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>19b0uaa</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>I finally went for a different shape 💓 I'm in love!</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1d023er8idc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>19b0fc8</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>How to prevent nails snapping/chipping</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19b0fc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>19b0280</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>I just love simple, white and sparkles.... Can I see your favorites please? 💅</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mt6uc8yv1idc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>19azzi5</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>It’s giving latte swirl ☕️</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hyfjm2m91idc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>19azygx</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>So glad I decided to put some effort into hand/nail care this past year!</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/isn86cr01idc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>19azthl</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>My Baby Blue Nails</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am3m9y2szhdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>19azt68</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Nail shape for dry, short, crooked wide, boney nails.</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19azt68</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>19azik4</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Dragon nails because, why not.</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5c4ztjg5xhdc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>19az5r6</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>What nail dryers do y’all recommend for gel?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19az5r6/what_nail_dryers_do_yall_recommend_for_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>19awygc</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Best nail length/shape for long fat giant hands lol?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hbuulpwchdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>19ax8w2</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>what do i say to get the pink chrome nails</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19ax8w2/what_do_i_say_to_get_the_pink_chrome_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>19ayw2d</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Tips/advice wanted</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ayw2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>19ayc1p</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Got my nails done for valentines day!</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ayc1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>19ax73z</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Nails! Did them myself</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejrw2o9oehdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>19ax4h0</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>I’m in love with this pink cat eye on almond 💕</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2wt4vh4ehdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>19awyhs</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Ombré on natural nails</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2zgd6fwchdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>19asw42</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>How to fix my cuticles/nails?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19asw42</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>19ary54</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Pink Ombré</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/01kyezggbgdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>19avnzh</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>My nails need someone to fix them</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2uzcji23hdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>19aub8k</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Trying out acrylic</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aub8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>19au6vi</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>My fav nude</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3em363f6sgdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>19au3py</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>finally found a good salon after a myriad of bad experiences 😭 what a good day</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q07luqrjrgdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>19au0ol</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>jumped on the baby pink chrome train 😇💖</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19au0ol</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>19ate1r</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>One of my newer polishes</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ate1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>19at7hk</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>OPI Nail envy for post-acrylic nails</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19at7hk/opi_nail_envy_for_postacrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>19asdak</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Had to cut them short for Bass Practice- definitely worth it</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19asdak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>19asbdb</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>i don’t wanna feel blue anymore, bluuuuuue 🎶</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19asbdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>19as4pf</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Can you extend your nail beds?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19as4pf/can_you_extend_your_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>19as23z</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Cuticula - Blue Flame</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19as23z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>19as08b</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Cuticula - Blue Flame</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19as08b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>19arxtx</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>One of my favorite nail art! 😈</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g5kdqtkebgdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>19arqzx</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Blue isn’t really my favorite, but I’m digging this</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19arqzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>19ar4m0</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>DND Wildflower: Much more taupe than the lacquer!</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqfr7obf5gdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>19aqzzm</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Robin eggs with stars</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/642m0w0h4gdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>19aq3gd</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Went with something simple today and love the way it turned out.</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7jbowvqxfdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>19aq37n</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Hearts 💕</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aq37n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>19apkqb</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>I’m so happy with the Holo Taco crackle. I hope she decides to make it in more colors.</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnecvahxtfdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>19ap2xg</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Second time at gel extensions!</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dusdev6dqfdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>19aog70</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>First time gel on natural nails</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aog70</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>19aog5v</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o63pz3nrlfdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>19aofqm</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Aren't they cute?!</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aofqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>19al3ji</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Making non-gel polish last on acrylics- please help!</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qe3ad74dwedc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>19al12p</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Inspired by the cold weather</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5pj46huvedc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>19ak9gq</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>gel polish peels immediately after shower, how to fix this?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19ak9gq/gel_polish_peels_immediately_after_shower_how_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>19aj13k</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>In love with my newest set (salon) ✨inspo pic by Estética Luciana found on Pinterest.</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aj13k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>19ao44f</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Would it be rude to ask for a manicure with no polish?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19ao44f/would_it_be_rude_to_ask_for_a_manicure_with_no/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>19any6y</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Does this shape suit my hands? I’m thinking of getting almond next time.</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8o83894ifdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>19anw96</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Finally did my nails after six months felt nice to get them done</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19anw96</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>19anfm4</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>wanted to hop onto the bow trend but i don’t think my nail girl was down for it 🎀🎀</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19anfm4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>19an5qu</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Blue Nail’s</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19an5qu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>19amz0o</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>2nd set of 2024</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5kmnrrxafdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>19amg3v</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>New Set for the New Year</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ga0qm237fdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>19ambal</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Gold ✨</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ambal</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>19am2zm</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Any way for me to add length getting acrylic fill?</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19am2zm/any_way_for_me_to_add_length_getting_acrylic_fill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>19alvk3</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19alvk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>19alppe</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>I really love my Nail Tech</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9d9haid1fdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>19allee</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Just discovered this sub! These are the nails I’ve done this year!(both good and bad)</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19allee</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>19aky37</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>🐆</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9oe9zsy6vedc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>19akw1i</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Wonky nails</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19akw1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>19ajshc</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>French</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwed46wdledc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>19ajeso</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Decided to ditch the almond shape for a change, and I love it!</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y07h44f7iedc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>19aj7uk</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>love my nail tech</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hpss8xkhgedc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>19aivo8</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Blueish purple chrome!!</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjqmu5ofdedc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>19aibe2</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Took off acrylics and tried something simple</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aibe2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>19ahx7z</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Early Valentine’s nails</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ahx7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>19aheub</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Birthday nails!! Baby pink chrome! I'm OBSESSED ♥️🥰</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aheub</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>19ah3e5</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>acrylics or gel x?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19ah3e5/acrylics_or_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>19agz3z</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Simple &amp; classy</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahnzkhultddc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>19af3sx</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Natural nails + nude shimmery polish💫</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrk7f4on6ddc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>19aeyni</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Do any of you have these bio colours ?</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19aeyni/do_any_of_you_have_these_bio_colours/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>19b6ie0</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Pinks keep me warm in the Colorado winter</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/t1ASRsw.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>19b5gxj</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>welp 🥲 this is 1/3 nails that were surviving on the teabag trick, I really don’t wanna go back to shorties….</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hiy0ks4gijdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>19b5gdj</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Obsessed 🌈✨</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19b5gdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>19b34ln</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Cuticula Limitless QDTC vs Vibrant Scents F&amp;H?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19b34ln/cuticula_limitless_qdtc_vs_vibrant_scents_fh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>19b2vua</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>KB Shimmer</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19b2vua/kb_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>19b2p07</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>First attempts decals and french tips</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19b2p07</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>19b2h2r</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>classic red feels so right for wintertime ❤️ (Sally Hansen ASAP Apple + Manucurist Green Flash Topcoat)</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19b2h2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>19b0vi4</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Yet another 'paperclip magnetized heart' mani</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c6vthndz8idc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>19azvhc</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>My Zoya 10 for $25 order arrived!</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pdj2r14b0idc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>19azued</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Finally swatched my whole collection (again) but now I can see everything!</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19azued</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>19azr2f</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Baby Blue Nails</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0pg3u44zhdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>19azoaz</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>My first set of Valentine’s nails OC</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19azoaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>19azd22</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Newbie looking for polish recommendations</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19azd22/newbie_looking_for_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>19azc2m</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>How do I completely remove the leftover blue?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19azc2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>19ayov0</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>A fitting end to a bad week</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ieb5xdaqhdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>19aykya</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Drip Drop feat. a rainy day in california</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s9i3txldphdc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>19aye11</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Bee’s knees drop is 15% off for everyone</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vngwjlunhdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>19aydv4</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Magnet hacks</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19aydv4/magnet_hacks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>19aycx5</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Disco nails for an event tonight!🪩🕺🏼🪩</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aycx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>19axgaq</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Sparkly nudes 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iz81mtglghdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>19axc79</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Just proud of myself...and thankful...</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aaf72h2qfhdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>19axa8l</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>They don’t sell my favorite base coat in the US. Are there any domestic polishes like this?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a18fslobfhdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>19awzym</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Orly - Prince Charming</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19awzym</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>19awpat</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Early Vday skittles</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4kaja50bhdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>19awobl</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Is it too late to discuss this? What are your nail polish goals for 2024?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkro712tahdc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>19awj31</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Update on Magnetics Success!</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4eqp1pq9hdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>19awgj0</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Slowly going through all of my thermals…</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19awgj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>19avloo</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>The Fitnessgram pacer test is a multistage aerobic capacity test that progressively gets more difficult as it continues...</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19avloo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>19avjgx</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Bee's Knees Lacquer offering 15% off everything tonight!!!</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19avjgx/bees_knees_lacquer_offering_15_off_everything/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>19avfh1</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>if frogs had wings</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19avfh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>19avb41</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>First attempt at velvet nails</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yowdt6xj0hdc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>19ava7z</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Finally searched my collection</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afztfowd0hdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>19av0ls</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Why do I get bubbles on my manicure? 😓</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0nj122fygdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>19aug4g</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Ombré on natural nails</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mppa1zt3ugdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>19aufym</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Essie Valentine’s Day Collection</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19aufym/essie_valentines_day_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>19aubis</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>When your team's going to the playoffs, you support them the best way you know how…</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aubis</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>19au5kw</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Polish Pickup order fulfillment time</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19au5kw/polish_pickup_order_fulfillment_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>19at24c</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Please ignore the fact that it’s actually not that smooth lmao</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrh87p1njgdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>19asmk5</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Springy little skittle because I am TIRED of being cold</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8n4otzhfggdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>19asf9k</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Zoya Skittles (I have jojoba oil on the way, I promise!)</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19asf9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>19asdho</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>You’re Not That Weird</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b3sa7r9gegdc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>19asb04</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>🥀🌹🍒 favourite set I’ve done so far :)</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtc510z1egdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>19as3gm</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Cuticula - Blue Flame</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19as3gm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>19arx8r</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Pastel Lavender</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19arx8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>19arerd</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Tasalon Professional Salon organizer</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19arerd/tasalon_professional_salon_organizer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>19aqvlh</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Hopping on the glow train!</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/td0cal7j3gdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>19aqpzm</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>What are your favorite "Granite" type polishes?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19aqpzm/what_are_your_favorite_granite_type_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>19aqg67</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Help IDing DVN shade (“Sticker Burr”?)</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aqg67</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>19aq96o</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Fine line filigree french (not pictured: all the ones I smeared).</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qomgltpyfdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>19apbl7</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Is there a brand you really want to love but just can't?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19apbl7/is_there_a_brand_you_really_want_to_love_but_just/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>19ap9su</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Plum with glitter</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/Eaj1roW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>19ap5rk</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>🏵 Klimt 🏵</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ap5rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>19aok7c</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>3D Printed “Mani Mags” vs. Regular Magnetic Wands</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aok7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>19anyje</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>quick dry polish for child</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19anyje/quick_dry_polish_for_child/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>19an499</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Has anyone used the Apres Beta LED lamp?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19an499/has_anyone_used_the_apres_beta_led_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>19an3xa</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>{PR} One word to describe this one?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1i4kxavxbfdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>19ams16</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Jellies have me sold!</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mo9tntna9fdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>19amo0n</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Seasonally Inappropriate 💅</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19amo0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>19am8p4</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Ignore the fact it looks like a cracked out child did my nails</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19am8p4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>19alt2q</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Germanikure</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19alt2q/germanikure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>19alrfn</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Snow and Glow</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19alrfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>19alqf5</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Terrazzo Nails</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19alqf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>19ak0c3</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Pinks with a blue flash are my favorite 😌 Dazzle Dry Beloved</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ak0c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>19ahtmf</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>The woooorst top coat</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8wxa83s2edc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>19aghw2</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>When do you ask a small indie about your order?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19aghw2/when_do_you_ask_a_small_indie_about_your_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>19ae9oo</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Back to work Feels :(</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ae9oo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>19b5qe4</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Had a fun time designing and making this set</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfmkvwgdljdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>19b4m71</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Im ready for Valentines Day🙌🏼</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zb73xax69jdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>19b3uwk</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Fun sets for this week✨</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19b3uwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>19b3smw</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>HELP!! Does any brand make a clear red acrylic nail powder?</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/19b3smw/help_does_any_brand_make_a_clear_red_acrylic_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>19azkb4</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Nailzkatkat full gel tips and her rubber base .</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19azkb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>19awpof</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Ombré pink on natural nails</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofsnw6j2bhdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>19apgs5</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Ombré pink on natural nails</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i86eoy44tfdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>19aneqx</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>💜✨</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19aneqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>19an4fo</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Tweed nails</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19an4fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>19alsy7</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Set by naildbymaya on IG</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojldoqw32fdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>19aknj7</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>🐆</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mep37jjqsedc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>19akh1b</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>💖</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19akh1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>19ahu5h</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Luffy👊Gear 5</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu3joqkr2edc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>19afiuf</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Making marble set is always my favorite</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ays2r1uxbddc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>19aecxt</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Butterfly nails to commemorate my fight with thyroid cancer (it’s called the butterfly gland, I no longer have mine)</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6eg6zt5xcdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jan 21 08:07:37 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_21.xlsx
+++ b/data/2024_01_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1135"/>
+  <dimension ref="A1:C1326"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19728,6 +19728,3253 @@
         </is>
       </c>
     </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>19by8ov</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Would you like a design like this for Valentine's Day?</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oy9rdecg0rdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>19by6rl</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Sparkly green</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2am2ooszqdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>19bx9e8</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Kuromi nails</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/092gfbdxoqdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>19bx6nt</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>cow nails 🤸</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wo1ijr41oqdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>19bx0ej</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>What color?</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgslxyk0mqdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>19bwrc3</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>which do we like better? for my birthday coming up, birthday dress is baby pink backless with a bow in the back</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bwrc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>19bwc6v</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Love my bow</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bwc6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>19bw6rk</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Pretty impressed with my home application. I’m autistic and struggle with nail salons, do they look okay?</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bw6rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>19bvtbt</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Love the new blue. Go get yourself some glitter.</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bvtbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>19bvf41</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>did my own biab nails 🩰</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9p62dv075qdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>19bvdlv</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Got the nails did, my first ever acrylic set</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bvdlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>19buzl6</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Lunar new year nails!! I love it🧧</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oknvg2tp0qdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>19buzbs</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>nail glue</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19buzbs/nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>19buljh</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbucly4lwpdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>19btwqq</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Cherry Blossoms 🌸</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19btwqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>19btm2r</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Stamping polish</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19btm2r/stamping_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>19bstsh</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>( *｀ω´)</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zno1gx3ffpdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>19bsgah</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Practicing my hearts</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bsgah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>19bs8u6</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Amazon soft gel tip press on ons! 🩷🩰</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bs8u6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>19bs8ov</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>is this okay for beginner</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aw23ybb4apdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>19bs6ns</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Favorite nails ever</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vizo8fk9pdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>19brz1b</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Valentine’s Nails</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxpdhu3l7pdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>19brpqe</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Cottagecore nails! (Pls don’t take down this month’s mods I don’t understand what I’m doing wrong)</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ci72mfld5pdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>19brksp</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Manucurist Paris Active Glow- updates?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19brksp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>19brja3</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>I cant get my gel X to stay on for over 3 days for the life of men</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19brja3/i_cant_get_my_gel_x_to_stay_on_for_over_3_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>19brcbk</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Pretty in Pink</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95nr3ub02pdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>19br6bw</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Just got these Gel X done 😍</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19br6bw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>19br206</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>GLOW UP</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19br206</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>19bqxpg</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Basic but I love them ✨</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bqxpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>19bqmex</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>4th at home gel manicure - slow but steady progress!</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kbybo2uvodc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>19bq6w2</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>What are these nails called?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gp5cskf5sodc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>19bq5tb</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>starting a gel journey</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19bq5tb/starting_a_gel_journey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>19bq4sg</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>This feels like it's serving The Birdcage aesthetics but I'm honestly so finished with this winter weather I'm leaning into the summer neons. LA Colors Gel / Rio, Maybelline Fast Gel / Orange Shot (I don't get the name on that last one, it's like a neon coral)</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofro4lwjrodc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>19bply8</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Scarab beetle nails!</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gysh3aubnodc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>19bp2mc</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>What do yall think about my nails?</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bp2mc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>19boiz9</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love my nail tech! </t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/el4l1kkleodc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>19bocp1</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>how did my nail tech do? 🥰</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rbs08gv8dodc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>19bobj0</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Natural Nails (even doing pottery!)</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ald87cbzcodc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>19boaz7</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>got a new nail polish! OPI “Lead by Example”</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4uzfpwucodc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>19bo3we</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>TikTok press ons</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bofudexbbodc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>19bnzun</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Simple snow nails</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bnzun</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>19bnp0l</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Simple nudes for my trip to company HQ.</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uea5vjqz7odc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>19bnm5s</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Good products for helping with nail growth?</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19bnm5s/good_products_for_helping_with_nail_growth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>19bnigm</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>I’m so proud of these</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bnigm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>19bnbwa</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Winter vibes ❄️</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2y3rhoe25odc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>19bn8lf</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Matte Black 🖤</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4sh7zyec4odc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>19bn5u2</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>my twist on valentine’s day nails! 🤍</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlr8d8bq3odc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>19bn0ce</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Got these nails done yesterday, I love them!</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bn0ce</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>19bmwli</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Playing the role of Classy this week</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckhfy3ip1odc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>19bmvst</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Black and white nails fantasy</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhpsb8ji1odc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>19bmo01</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8iux4iuzndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>19bmnbf</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Just felt like something a bit more subdued today. Irina @ lashnnail room hit it out of the park!!</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bmnbf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>19blye5</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>dip chipping after 1 week?</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19blye5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>19blrtx</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Freestyle</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/noens0zvsndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>19blnm9</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2ep4v5zrndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>19bllij</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Last years birthday nails 💖🌸🎀</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1soarehrndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>19bll9n</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Snow nails!</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ps3u99bfrndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>19blc77</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Is this ok? Got them done for the first time</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19blc77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>19bl6lu</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Is this a good neutral/pinkish colour for my skin tone?</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o89egvz8ondc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>19bl50d</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>new nails</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bl50d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>19bks1x</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>baby pink 🩰</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bks1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>19bkp2f</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>💜💜</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oily06hfkndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>19bk77t</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>New Years &amp; Winter Wonderland nails</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bk77t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>19bk4v1</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Newest set I’m working on! Opinions?</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zgv5jx3gndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>19bjzj1</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>hype these up please</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flis0tmxendc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>19bjius</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>I’m blue dabadee</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bjius</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>19bj3qp</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Beginner nails PT. 3</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bj3qp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>19bj3kg</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Just a little Valentine’s set 🩷💌</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kvsgnx18ndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>19bj3jh</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Gold foil nails</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smpp9yh18ndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>19bivtv</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Best reflective glitter polish brands?</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bivtv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>19biq53</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>New favorite color, I think.</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xttvft8a5ndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>19bhw07</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Why is it when you get a "pink and white" acrylic manicure, the nail techs re-do a full set instead of a fill in?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/px1yudjuymdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>19bhvsz</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Where to buy gel polish?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19bhvsz/where_to_buy_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>19bhm1m</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>im trying to grow out my nails, what do i do with the nails i have?</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bhm1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>19bhpdb</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Valentines set 💖</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bhpdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>19bglsd</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Rhinestones fell off my nail :,)</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fb15lcitomdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>19bfndk</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Valentine kitty set</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bfndk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>19bdx5q</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>What am i doing wrong that causes the paint to just lift off completely? I know my work is rough them, but i can usualy get 3 or 4 days before chipping starts. Never had whole nails fall off.</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bdx5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>19bc177</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Can my nails be saved in the long term?</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vj3yvfomldc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>19bb7rp</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>I took inspo from a post on here but can’t remember who the OP was, I love them! So thanks!</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjxmtg1ueldc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>19baut5</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>My boyfriend broke up with me, so I tried fixing my broken heart with kintsugi inspired nails</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19baut5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>19bgs0d</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Is this color suiting my skin tone?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dikk3y5qmdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>19bg4kf</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Kinda regret doing these for my birthday... My boss thought my nails were chipped 🙃</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bg4kf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>19bfmg3</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Todays client!</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spmqt7y2hmdc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>19bfl3p</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>First time using builder gel</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97n1ztgsgmdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>19bfgfh</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Is it to early for Valentine's nails??</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19bfgfh/is_it_to_early_for_valentines_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>19bfcu7</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Ravenclaw nails</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/582h6fxzemdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>19bfaly</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Had to share this mani 🩷</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjq0xngiemdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>19bf9lc</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>I just realized I charge this custom design way too low mid way 🥹</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bf9lc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>19bf9cl</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Home "salon" gift</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19bf9cl/home_salon_gift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>19bentl</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>I Love This Pink</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x6jmm5ch9mdc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>19bek4k</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Press on question</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19bek4k/press_on_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>19bdtac</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>What shape to choose?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bdtac</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>19bdrj0</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>🥲 been trying to grow mine out then this happens</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lm3kemd12mdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>19bdoj5</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>On the ILNP bandwagon</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imwiarwc1mdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>19bdhbx</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Dip powder vs Gel: What is your preferred method and why?</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1kkhiwozldc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>19bcsck</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bcsck</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>19bchv1</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Super Mario Kart. Fun set done by my nail tech. My kitty approves</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bchv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>19bbrp7</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>💖</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8ekc6m7kldc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>19b9p7v</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>The second set I've ever done on myself and I'm so proud! Also please look at them with the camera flash on 🤩 Any feedback for improvement welcome 🥰</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19b9p7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>19bxg4z</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>ISO this mystery polish</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91dv0hk1rqdc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>19bwjlo</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Where is everyone’s fave place/brand to buy crème colours from? Needing to build up my collection of crème polishes.</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19bwjlo/where_is_everyones_fave_placebrand_to_buy_crème/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>19bw4db</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Scarab beetle nails!🪲</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/477sl7lecqdc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>19bvxvy</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>HELP! can I salvage this?!??</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bvxvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>19bvqdx</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>A nice palette cleanser 🖤</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bvqdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>19bvn8o</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Surprise cats!</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bvn8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>19buuqp</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Mooncat Outlaw Country</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19buuqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>19buo9p</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Valentine’s Day ready!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ceiy4ukexpdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>19bumje</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Do You Play Croquet? Mooncat w/ 9D Topper</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bumje</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>19buk1n</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Switching to doing my own nails- how long does regular nail polish last?</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19buk1n/switching_to_doing_my_own_nails_how_long_does/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>19bu5qi</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>I need spring 😂😭</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bu5qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>19bu4vs</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Purple frost</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bu4vs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>19btyf2</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Can you guess this polish?</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19btyf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>19btpqo</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Colors arrived!</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rt2f3kfsnpdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>19btlrb</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Tried comic book nails for the first time today!</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19btlrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>19bsz2x</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>I did this nail art today but I'm not sure if it good enough? what do you think?any advice?</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqr3v09rgpdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>19bsmc2</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Crazy Cat Lady</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bsmc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>19bsaom</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>My recent nail set</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nrjuatvlapdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>19bs8y2</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>This one is so dreamy…</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bs8y2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>19bs6zh</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>New polish joys</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bs6zh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>19brumf</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Successfully avoided flooding cuticles!</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19brumf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>19bra8r</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>This better not be nail polish</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vsbdakh1pdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>19br8yr</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Rainshower by ILNP</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19br8yr/rainshower_by_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>19br19f</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>First time trying marble nails</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19br19f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>19bqk2c</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>What's less likely to give me an allergy: acrylics or builder gel?</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19bqk2c/whats_less_likely_to_give_me_an_allergy_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>19bqhpn</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Heart magnet hack!</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tqe4il3nuodc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>19bqajf</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>4th at home gel manicure - slow but steady progress!</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9z72elxysodc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>19boyvm</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Swatched my collection today 💅</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19boyvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>19bo5yv</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Simple snow nails</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bo5yv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>19bo54h</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Recommendations for any polishes that will give this color?</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bo54h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>19bo1ks</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Love iridescent nails</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cys14etaodc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>19bo1cv</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>🍉 🍉🍉</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ret0okrraodc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>19bn4hn</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Happy with my new mani</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bn4hn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>19bmwb3</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>🐉 Ether Dragon! 🐉</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ai50fprh1odc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>19bmi2f</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Orly, Zoya, OPI, or Essie?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19bmi2f/orly_zoya_opi_or_essie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>19bmg0y</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Magnet Hack 🧲 Jewelry Box Edition</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bmg0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>19bm5u5</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Vibrant Scents base coat alternative?</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4mbxexwvndc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>19blz92</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>ILNP Sleigh Bells</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ce3hmwggundc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>19blvdo</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Polishes like ILNP Moondust</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19blvdo/polishes_like_ilnp_moondust/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>19blihh</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Found an old bottle of magnetic nail polish (probably from the early 2010's) and I don't hate it</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t22sjt5uqndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>19bl2lp</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First magnetic polish - Mooncat Weeping Willow </t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uta9lneenndc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>19bkvls</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Drown my demons 🌊</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7b1sb5wtlndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>19bkpvp</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>question about dermatitis from gel</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19bkpvp/question_about_dermatitis_from_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>19bkfsm</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>ABCs of polish! M is for Monarch Lacquer</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13e8x5mfindc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>19bjudi</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Sally Hansen New Atti-hue</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bjudi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>19bjijn</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>My new favorite - SO MANY COLORS</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kkc3vsk1bndc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>19bja2s</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>LynB - If it fits I sits</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bja2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>19bj39h</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>🍫 Looking Like Dessert 🍩</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bj39h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>19bj0z7</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Do you mix your polishes?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rs2gy6d7ndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>19biyqp</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>I wanted to do a different purple mani on each hand 💜</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3r3h6i37ndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>19biwpy</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>self care saturday calls for a new manicure 🥰</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19biwpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>19biqom</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Community Question</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19biqom/community_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>19biic7</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Soft pink vibes</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19biic7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>19bhz6g</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Matte Black 🖤</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0sxzd8jzmdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>19bhtjl</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Best places to buy quality gel polish in Canada?</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19bhtjl/best_places_to_buy_quality_gel_polish_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>19bhqdx</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Hand painted Valentines set 💖</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bhqdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>19bh8o6</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>✨️Existential Crisis ✨️</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bh8o6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>19bh2yj</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Air bubbles in top coat?</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bh2yj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>19bh02d</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Morticia’s Pup Cup - Zombie Claw</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqcoc9tyrmdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>19bgs9u</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Need a reco</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19bgs9u/need_a_reco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>19bgmgv</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Holo Taco - Play Rosé</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bgmgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>19bgeya</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Dupe for my fave vintage polish?</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bgeya</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>19bg1hp</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Trying to get the best out of my natural nails, but am insecure bc they aren't really symmetrical. Do they look presentable without nail polish? 🙈</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bg1hp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>19bf935</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Presenting my Birthday Set! 🎉</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bf935</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>19bf16i</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Fairy Dust is my new favorite!</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bf16i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>19betq9</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>My first Beaux Rêves polish</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c33e53qsamdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>19bebdw</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>deep space love 🌌</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bebdw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>19be621</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Does anyone know what this effect is called &amp; how it is created with cat eye gel?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19be621</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>19bdkza</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hc7jqe6l0mdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>19bdefo</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>What's your all-time favorite white pearl nail polish?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19bdefo/whats_your_alltime_favorite_white_pearl_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>19bdaz6</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Longest they have ever been!</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bdaz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>19bdadk</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Holo Taco VS Mooncat</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19bdadk/holo_taco_vs_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>19bd95j</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Brittle nail treatments please!</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19bd95j/brittle_nail_treatments_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>19bcv00</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Galaxy nails I did with regular polish 🌌</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4t7cmuculdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>19bbcwb</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Current Indie Brands Similar to Nerd Lacquer, Hare Polish, and Scofflaw?</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19bbcwb/current_indie_brands_similar_to_nerd_lacquer_hare/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>19bawxn</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Please help me understand my cuticles</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bawxn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>19b4xcm</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Dazzle dry?</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19b4xcm/dazzle_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>19b77jy</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Star sapphire vibes 💎</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yseb3blz2kdc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>19byddu</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Would you like a design like this for Valentine's Day?</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2apxnjm42rdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>19bwixg</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Gold and white is always my favorite!</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwwg5xaogqdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>19butv0</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>First time doing acrylics</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19butv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>19bu0kn</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>My friend got his first manicure today :)</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmc1bptpqpdc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>19bq44q</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Pink Scream theme</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2l3q1iirodc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>19bp81d</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>New member</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enu85bt4kodc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>19bp1zl</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Anyone got tips so there are no strokes in the silver nail polish?⭐️⭐️</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6w6nfstiodc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>19bk98l</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Cosmic nails with 3 types of cat eye</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9m2eh81hndc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>19bhonq</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Valentines set 💖</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bhonq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>19bhgf3</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Monster press ons.</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vrkhx4kvmdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>19bfmir</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Valentine kitty set</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19bfmir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>19bfa57</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Ravenclaw nails</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djntb1ffemdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>19bbr7y</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Waiting for Spring</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvwb8m43kldc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>